<commit_message>
fix not to use sheets and refactoring
</commit_message>
<xml_diff>
--- a/test.xls.xlsx
+++ b/test.xls.xlsx
@@ -4,8 +4,6 @@
   <workbookPr date1904="false"/>
   <sheets>
     <sheet name="構造体一覧" sheetId="1" r:id="rId4"/>
-    <sheet name="Test00" sheetId="2" r:id="rId5"/>
-    <sheet name="Test01" sheetId="3" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
@@ -16,7 +14,7 @@
     <numFmt numFmtId="100" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="101" formatCode="yyyy/mm/dd hh:mm:ss"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <name val="Arial"/>
       <sz val="11"/>
@@ -27,6 +25,11 @@
       <sz val="20"/>
       <family val="1"/>
       <b val="true"/>
+    </font>
+    <font>
+      <name val="ＭＳ Ｐゴシック"/>
+      <sz val="10"/>
+      <family val="1"/>
     </font>
     <font>
       <name val="ＭＳ Ｐゴシック"/>
@@ -101,15 +104,18 @@
   <cellStyleXfs count="1">
     <xf borderId="0" numFmtId="0" fontId="0" fillId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" numFmtId="0" fontId="0" fillId="0" xfId="0"/>
     <xf borderId="1" numFmtId="0" fontId="0" fillId="0" xfId="0"/>
     <xf borderId="0" numFmtId="14" fontId="0" fillId="0" xfId="0" applyNumberFormat="1"/>
     <xf borderId="0" numFmtId="0" fontId="1" fillId="0" applyNumberFormat="false" applyFill="false" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf borderId="2" numFmtId="0" fontId="2" fillId="2" applyNumberFormat="false" applyFill="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf borderId="0" numFmtId="0" fontId="2" fillId="0" applyNumberFormat="false" applyFill="false" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" wrapText="true"/>
+    </xf>
+    <xf borderId="2" numFmtId="0" fontId="3" fillId="2" applyNumberFormat="false" applyFill="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf borderId="3" numFmtId="0" fontId="3" fillId="0" applyNumberFormat="false" applyFill="false" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf borderId="3" numFmtId="0" fontId="4" fillId="0" applyNumberFormat="false" applyFill="false" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -126,82 +132,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="5"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="30"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="30"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="3" t="inlineStr">
-        <is>
-          <t>構造体一覧</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="inlineStr">
-        <is>
-          <t>No.</t>
-        </is>
-      </c>
-      <c r="B2" s="4" t="inlineStr">
-        <is>
-          <t>構造体名</t>
-        </is>
-      </c>
-      <c r="C2" s="4" t="inlineStr">
-        <is>
-          <t>備考</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="5" t="str">
-        <f>HYPERLINK("#Test00!A1","Test00")</f>
-      </c>
-      <c r="C3" s="5" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5" t="str">
-        <f>HYPERLINK("#Test01!A1","Test01")</f>
-      </c>
-      <c r="C4" s="5" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <sheetCalcPr fullCalcOnLoad="true"/>
-  <printOptions verticalCentered="false" horizontalCentered="false" headings="false" gridLines="false"/>
-  <pageMargins right="0.75" left="0.75" bottom="1.0" top="1.0" footer="0.5" header="0.5"/>
-  <pageSetup/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <sheetPr>
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:A26"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -216,302 +147,397 @@
     <row r="1">
       <c r="A1" s="3" t="inlineStr">
         <is>
+          <t>構造体一覧</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="5" t="inlineStr">
+        <is>
+          <t>No.</t>
+        </is>
+      </c>
+      <c r="B2" s="5" t="inlineStr">
+        <is>
+          <t>構造体名</t>
+        </is>
+      </c>
+      <c r="C2" s="5" t="inlineStr">
+        <is>
+          <t>備考</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="str">
+        <f>HYPERLINK("#A6","Test00")</f>
+      </c>
+      <c r="C3" s="6" t="inlineStr">
+        <is>
+          <t>テスト００のデータ構造</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6" t="str">
+        <f>HYPERLINK("#A16","Test01")</f>
+      </c>
+      <c r="C4" s="6" t="inlineStr">
+        <is>
+          <t>テスト０１のデータ構造</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
           <t>Test00構造体</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="4" t="inlineStr">
+    <row r="7">
+      <c r="A7" s="4" t="inlineStr">
+        <is>
+          <t>概要：</t>
+        </is>
+      </c>
+      <c r="B7" s="4" t="inlineStr">
+        <is>
+          <t>テスト００のデータ構造</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="inlineStr">
+        <is>
+          <t>詳細：</t>
+        </is>
+      </c>
+      <c r="B8" s="4" t="inlineStr">
+        <is>
+          <t>この構造は最大長を考慮して定義してある</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="5" t="inlineStr">
         <is>
           <t>No.</t>
         </is>
       </c>
-      <c r="B2" s="4" t="inlineStr">
+      <c r="B9" s="5" t="inlineStr">
         <is>
           <t>メンバ型</t>
         </is>
       </c>
-      <c r="C2" s="4" t="inlineStr">
+      <c r="C9" s="5" t="inlineStr">
         <is>
           <t>メンバ変数名</t>
         </is>
       </c>
-      <c r="D2" s="4" t="inlineStr">
+      <c r="D9" s="5" t="inlineStr">
         <is>
           <t>備考</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="5" t="n">
+    <row r="10">
+      <c r="A10" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="inlineStr">
+      <c r="B10" s="6" t="inlineStr">
         <is>
           <t>bool</t>
         </is>
       </c>
-      <c r="C3" s="5" t="inlineStr">
+      <c r="C10" s="6" t="inlineStr">
         <is>
           <t>member00</t>
         </is>
       </c>
-      <c r="D3" s="5" t="inlineStr">
+      <c r="D10" s="6" t="inlineStr">
         <is>
           <t>メンバー００</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="5" t="n">
+    <row r="11">
+      <c r="A11" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="5" t="inlineStr">
+      <c r="B11" s="6" t="inlineStr">
         <is>
           <t>unsigned char</t>
         </is>
       </c>
-      <c r="C4" s="5" t="inlineStr">
+      <c r="C11" s="6" t="inlineStr">
         <is>
           <t>member01</t>
         </is>
       </c>
-      <c r="D4" s="5" t="inlineStr">
+      <c r="D11" s="6" t="inlineStr">
         <is>
           <t>メンバー０１</t>
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="5" t="n">
+    <row r="12">
+      <c r="A12" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="inlineStr">
+      <c r="B12" s="6" t="inlineStr">
         <is>
           <t>short</t>
         </is>
       </c>
-      <c r="C5" s="5" t="inlineStr">
+      <c r="C12" s="6" t="inlineStr">
         <is>
           <t>member02</t>
         </is>
       </c>
-      <c r="D5" s="5" t="inlineStr">
+      <c r="D12" s="6" t="inlineStr">
         <is>
           <t>メンバー０２</t>
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="5" t="n">
+    <row r="13">
+      <c r="A13" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="5" t="inlineStr">
+      <c r="B13" s="6" t="inlineStr">
         <is>
           <t>unsigned short</t>
         </is>
       </c>
-      <c r="C6" s="5" t="inlineStr">
+      <c r="C13" s="6" t="inlineStr">
         <is>
           <t>member03</t>
         </is>
       </c>
-      <c r="D6" s="5" t="inlineStr">
+      <c r="D13" s="6" t="inlineStr">
         <is>
           <t>メンバー０３</t>
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="5" t="n">
+    <row r="14">
+      <c r="A14" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="5" t="inlineStr">
+      <c r="B14" s="6" t="inlineStr">
         <is>
           <t>int</t>
         </is>
       </c>
-      <c r="C7" s="5" t="inlineStr">
+      <c r="C14" s="6" t="inlineStr">
         <is>
           <t>member04</t>
         </is>
       </c>
-      <c r="D7" s="5" t="inlineStr">
+      <c r="D14" s="6" t="inlineStr">
         <is>
           <t>メンバー０４</t>
         </is>
       </c>
     </row>
-  </sheetData>
-  <sheetCalcPr fullCalcOnLoad="true"/>
-  <printOptions verticalCentered="false" horizontalCentered="false" headings="false" gridLines="false"/>
-  <pageMargins right="0.75" left="0.75" bottom="1.0" top="1.0" footer="0.5" header="0.5"/>
-  <pageSetup/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <sheetPr>
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:D8"/>
-  <sheetViews>
-    <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="5"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="50"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="50"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="50"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="3" t="inlineStr">
+    <row r="15">
+      <c r="A15" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="inlineStr">
         <is>
           <t>Test01構造体</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="4" t="inlineStr">
+    <row r="17">
+      <c r="A17" s="4" t="inlineStr">
+        <is>
+          <t>概要：</t>
+        </is>
+      </c>
+      <c r="B17" s="4" t="inlineStr">
+        <is>
+          <t>テスト０１のデータ構造</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="4" t="inlineStr">
+        <is>
+          <t>詳細：</t>
+        </is>
+      </c>
+      <c r="B18" s="4" t="inlineStr">
+        <is>
+          <t>１行目
+２行目
+３行目</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="5" t="inlineStr">
         <is>
           <t>No.</t>
         </is>
       </c>
-      <c r="B2" s="4" t="inlineStr">
+      <c r="B19" s="5" t="inlineStr">
         <is>
           <t>メンバ型</t>
         </is>
       </c>
-      <c r="C2" s="4" t="inlineStr">
+      <c r="C19" s="5" t="inlineStr">
         <is>
           <t>メンバ変数名</t>
         </is>
       </c>
-      <c r="D2" s="4" t="inlineStr">
+      <c r="D19" s="5" t="inlineStr">
         <is>
           <t>備考</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="5" t="n">
+    <row r="20">
+      <c r="A20" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="inlineStr">
+      <c r="B20" s="6" t="inlineStr">
         <is>
           <t>bool</t>
         </is>
       </c>
-      <c r="C3" s="5" t="inlineStr">
+      <c r="C20" s="6" t="inlineStr">
         <is>
           <t>member10</t>
         </is>
       </c>
-      <c r="D3" s="5" t="inlineStr">
+      <c r="D20" s="6" t="inlineStr">
         <is>
           <t>メンバー１０</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="5" t="n">
+    <row r="21">
+      <c r="A21" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="5" t="inlineStr">
+      <c r="B21" s="6" t="inlineStr">
         <is>
           <t>unsigned char</t>
         </is>
       </c>
-      <c r="C4" s="5" t="inlineStr">
+      <c r="C21" s="6" t="inlineStr">
         <is>
           <t>member11</t>
         </is>
       </c>
-      <c r="D4" s="5" t="inlineStr">
+      <c r="D21" s="6" t="inlineStr">
         <is>
           <t>メンバー１１</t>
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="5" t="n">
+    <row r="22">
+      <c r="A22" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="inlineStr">
+      <c r="B22" s="6" t="inlineStr">
         <is>
           <t>short</t>
         </is>
       </c>
-      <c r="C5" s="5" t="inlineStr">
+      <c r="C22" s="6" t="inlineStr">
         <is>
           <t>member12</t>
         </is>
       </c>
-      <c r="D5" s="5" t="inlineStr">
+      <c r="D22" s="6" t="inlineStr">
         <is>
           <t>メンバー１２</t>
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="5" t="n">
+    <row r="23">
+      <c r="A23" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="5" t="inlineStr">
+      <c r="B23" s="6" t="inlineStr">
         <is>
           <t>unsigned short</t>
         </is>
       </c>
-      <c r="C6" s="5" t="inlineStr">
+      <c r="C23" s="6" t="inlineStr">
         <is>
           <t>member13</t>
         </is>
       </c>
-      <c r="D6" s="5" t="inlineStr">
+      <c r="D23" s="6" t="inlineStr">
         <is>
           <t>メンバー１３</t>
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="5" t="n">
+    <row r="24">
+      <c r="A24" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="5" t="inlineStr">
+      <c r="B24" s="6" t="inlineStr">
         <is>
           <t>int</t>
         </is>
       </c>
-      <c r="C7" s="5" t="inlineStr">
+      <c r="C24" s="6" t="inlineStr">
         <is>
           <t>member14</t>
         </is>
       </c>
-      <c r="D7" s="5" t="inlineStr">
+      <c r="D24" s="6" t="inlineStr">
         <is>
           <t>メンバー１４</t>
         </is>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="5" t="n">
+    <row r="25">
+      <c r="A25" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="5" t="str">
-        <f>HYPERLINK("#Test00!A1","Test00")</f>
-      </c>
-      <c r="C8" s="5" t="inlineStr">
+      <c r="B25" s="6" t="str">
+        <f>HYPERLINK("#A6","Test00")</f>
+      </c>
+      <c r="C25" s="6" t="inlineStr">
         <is>
           <t>member15</t>
         </is>
       </c>
-      <c r="D8" s="5" t="inlineStr">
+      <c r="D25" s="6" t="inlineStr">
         <is>
           <t>メンバー１５</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="inlineStr">
+        <is>
+          <t/>
         </is>
       </c>
     </row>

</xml_diff>